<commit_message>
add panel progress and material template import
</commit_message>
<xml_diff>
--- a/public/assets/excel-templates/imports/progress-raw-materials/progress-raw-material-import.xlsx
+++ b/public/assets/excel-templates/imports/progress-raw-materials/progress-raw-material-import.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Laravel-proc\rekachain-web\public\assets\excel-templates\imports\progress-raw-materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7429170F-C663-4E47-B8F5-DF385938E0F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789F2824-8EE1-4537-8C52-4886C7642628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="345" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Material" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Deskripsi</t>
   </si>
@@ -40,15 +40,9 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Specs</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>Kode</t>
-  </si>
-  <si>
     <t>22B58OH00000XXG01</t>
   </si>
   <si>
@@ -85,13 +79,28 @@
     <t>Nama Proses</t>
   </si>
   <si>
+    <t>Bending</t>
+  </si>
+  <si>
+    <t>QC Cutting &amp; Bending</t>
+  </si>
+  <si>
+    <t>Spesifikasi</t>
+  </si>
+  <si>
+    <t>Kode Material</t>
+  </si>
+  <si>
+    <t>Pemotongan Bahan</t>
+  </si>
+  <si>
+    <t>Penganuan Bahan</t>
+  </si>
+  <si>
+    <t>Pengecekan Kualitas Pemotongan dan Penganuan Barang</t>
+  </si>
+  <si>
     <t>Cutting</t>
-  </si>
-  <si>
-    <t>Bending</t>
-  </si>
-  <si>
-    <t>QC Cutting &amp; Bending</t>
   </si>
 </sst>
 </file>
@@ -180,9 +189,9 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F492DBDB-7A24-4E92-82BD-C1CF5C545CD2}" name="Kode"/>
+    <tableColumn id="1" xr3:uid="{F492DBDB-7A24-4E92-82BD-C1CF5C545CD2}" name="Kode Material"/>
     <tableColumn id="2" xr3:uid="{3E458159-F364-425D-AC5D-7FD0A56D745C}" name="Deskripsi"/>
-    <tableColumn id="3" xr3:uid="{1A219B18-F10B-4119-BEAE-5ECAEECD2FCC}" name="Specs"/>
+    <tableColumn id="3" xr3:uid="{1A219B18-F10B-4119-BEAE-5ECAEECD2FCC}" name="Spesifikasi"/>
     <tableColumn id="4" xr3:uid="{AFA89BA6-BA41-40C9-9D51-AA7FA942D57F}" name="Unit"/>
     <tableColumn id="5" xr3:uid="{3F83E40A-D01E-499D-A480-DB5AC5796DB1}" name="Qty"/>
   </tableColumns>
@@ -191,16 +200,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EBA50A7-FE7B-4694-9173-576F5386F178}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B4" xr:uid="{217FAAA6-2252-4C8D-A158-060B57A62051}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EBA50A7-FE7B-4694-9173-576F5386F178}" name="Table2" displayName="Table2" ref="A1:C4" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C4" xr:uid="{217FAAA6-2252-4C8D-A158-060B57A62051}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{18D610D8-81B3-4343-8B54-02F3A3EB617D}" name="Urutan">
       <calculatedColumnFormula>ROW()-ROW(Table2[[#Headers],[Urutan]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{B4B3E70E-BACA-47F7-9D7C-35164148A046}" name="Nama Proses"/>
+    <tableColumn id="3" xr3:uid="{2DA4E1DE-BBC8-4C19-8C43-2AB785A23093}" name="Deskripsi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,10 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE32E34-A79C-4932-8226-A755532272E7}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,33 +532,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -554,16 +566,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -571,16 +583,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -601,57 +613,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923E7235-3EB5-4A44-864C-0FA0334CD606}">
-  <dimension ref="A1:B4"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>ROW()-ROW(Table2[[#Headers],[Urutan]])</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>ROW()-ROW(Table2[[#Headers],[Urutan]])</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>ROW()-ROW(Table2[[#Headers],[Urutan]])</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>